<commit_message>
Added Update Test for Stripe API
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/Exceldata.xlsx
+++ b/src/test/resources/ExcelData/Exceldata.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\John\Learnings\ApiTestingFramework\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\John\Projects\ApiTestingFramework\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -71,14 +72,239 @@
     <t>cus_Hia93QPJFJcpEJ</t>
   </si>
   <si>
-    <t>cus_HicmBFfrkHgC9u</t>
+    <t>cus_HjN0KbwW3PQg8W</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>cus_HjN0iFS8Grw9GQ</t>
+  </si>
+  <si>
+    <t>cus_HjMwOChJOg2fae</t>
+  </si>
+  <si>
+    <t>cus_HjMwhRBgd2ZZXY</t>
+  </si>
+  <si>
+    <t>cus_HjFhFohCcSi8Wj</t>
+  </si>
+  <si>
+    <t>cus_HjFhgdGHycv84R</t>
+  </si>
+  <si>
+    <t>cus_HjFQKESdMqG0Nu</t>
+  </si>
+  <si>
+    <t>cus_HjFQx0hUypH8v1</t>
+  </si>
+  <si>
+    <t>cus_HjFQkjYktBQ9Ed</t>
+  </si>
+  <si>
+    <t>cus_HjFQkz483Gro1t</t>
+  </si>
+  <si>
+    <t>cus_HjF6v19n45fBF8</t>
+  </si>
+  <si>
+    <t>cus_HjF6xx6X6lVzBM</t>
+  </si>
+  <si>
+    <t>cus_HjF6WOCMuWlaYf</t>
+  </si>
+  <si>
+    <t>cus_HjF6OwszYsvm62</t>
+  </si>
+  <si>
+    <t>cus_HjEx2B7I3Pnl81</t>
+  </si>
+  <si>
+    <t>cus_HjExW2PB0odEp0</t>
+  </si>
+  <si>
+    <t>cus_HjEvclcfcjykA5</t>
+  </si>
+  <si>
+    <t>cus_HjEvXFbDLF3cY1</t>
+  </si>
+  <si>
+    <t>cus_HjEqgTbVl2meiM</t>
+  </si>
+  <si>
+    <t>cus_HjEqdTRye7Zpjx</t>
+  </si>
+  <si>
+    <t>cus_HjEp8BmoRtLd30</t>
+  </si>
+  <si>
+    <t>cus_HjEpSqcFeURpqT</t>
+  </si>
+  <si>
+    <t>cus_HjEoZkfRE1IBwL</t>
+  </si>
+  <si>
+    <t>cus_HjEoD4wepdcn80</t>
+  </si>
+  <si>
+    <t>cus_HjEnukocmEkMvK</t>
+  </si>
+  <si>
+    <t>cus_HjEnISjsiLH1sC</t>
+  </si>
+  <si>
+    <t>cus_HjEn0NdtyMsCL8</t>
+  </si>
+  <si>
+    <t>cus_HjEnhAcvpCKRX7</t>
+  </si>
+  <si>
+    <t>cus_HjEMwrzolYdEPR</t>
+  </si>
+  <si>
+    <t>cus_HjEM0LBbbpa7jt</t>
+  </si>
+  <si>
+    <t>cus_HjEKxQ0O4SW9J1</t>
+  </si>
+  <si>
+    <t>cus_HjEKNT5VkdRxrc</t>
+  </si>
+  <si>
+    <t>cus_Higg9ScqgBg6cX</t>
+  </si>
+  <si>
+    <t>cus_HiggOF0dhJqIDK</t>
+  </si>
+  <si>
+    <t>cus_HigfcEk887iasX</t>
+  </si>
+  <si>
+    <t>cus_HigfA5w5JhYFNS</t>
+  </si>
+  <si>
+    <t>cus_HigejemrOFkrp7</t>
+  </si>
+  <si>
+    <t>cus_Hige8DE1kXOR0a</t>
+  </si>
+  <si>
+    <t>cus_HigW6CubndTTeR</t>
+  </si>
+  <si>
+    <t>cus_HigWuvrylPU8PO</t>
+  </si>
+  <si>
+    <t>cus_HigKfP1qdgfrJ0</t>
+  </si>
+  <si>
+    <t>cus_HigKtrEyVLiqte</t>
+  </si>
+  <si>
+    <t>cus_HigJ9zApcJSP8r</t>
+  </si>
+  <si>
+    <t>cus_HigJy5KL9CYdiA</t>
+  </si>
+  <si>
+    <t>cus_HigIRfMW6o7gib</t>
+  </si>
+  <si>
+    <t>cus_HigIU2dGLdkIbz</t>
+  </si>
+  <si>
+    <t>cus_HigI7KCinB8Djk</t>
+  </si>
+  <si>
+    <t>cus_HigI55uumrKp4B</t>
+  </si>
+  <si>
+    <t>cus_HicmcUkqrPAPPl</t>
+  </si>
+  <si>
+    <t>cus_Hib0tlQuQGl8IQ</t>
+  </si>
+  <si>
+    <t>cus_HiWCHlD1ohK7TC</t>
+  </si>
+  <si>
+    <t>cus_HiW69F322JfDjh</t>
+  </si>
+  <si>
+    <t>cus_HiW6yOjUoqVnH6</t>
+  </si>
+  <si>
+    <t>cus_HiVvTXRM2mEpz8</t>
+  </si>
+  <si>
+    <t>cus_HiVvjP7NkYFIm8</t>
+  </si>
+  <si>
+    <t>cus_HiVvXyRIf1SypJ</t>
+  </si>
+  <si>
+    <t>cus_HiVnUVwVDJUrOr</t>
+  </si>
+  <si>
+    <t>cus_HiVnfBs6bNmspk</t>
+  </si>
+  <si>
+    <t>cus_HiVint2B7usItB</t>
+  </si>
+  <si>
+    <t>cus_HiVid9a9CHp1pA</t>
+  </si>
+  <si>
+    <t>cus_HiVfiM7Kiurkha</t>
+  </si>
+  <si>
+    <t>cus_HiVfsIOejD2qp2</t>
+  </si>
+  <si>
+    <t>cus_HiVZ309sVxkkrm</t>
+  </si>
+  <si>
+    <t>cus_HiVZau95ZSGCke</t>
+  </si>
+  <si>
+    <t>cus_HiVXzhXRgrDSQQ</t>
+  </si>
+  <si>
+    <t>cus_HiVXyxWCtKzPHm</t>
+  </si>
+  <si>
+    <t>cus_HhvNlkreZBiDvZ</t>
+  </si>
+  <si>
+    <t>cus_HhvM9zrAXAT88L</t>
+  </si>
+  <si>
+    <t>cus_HhvMp1oLfXUQyK</t>
+  </si>
+  <si>
+    <t>cus_Hh97GfMm6VOm3M</t>
+  </si>
+  <si>
+    <t>cus_Hh97IJgXiqE1QH</t>
+  </si>
+  <si>
+    <t>cus_Hh8ZMfRC4PZJBH</t>
+  </si>
+  <si>
+    <t>cus_Hh8ZtGdNv1hsiR</t>
+  </si>
+  <si>
+    <t>updateCustomers</t>
+  </si>
+  <si>
+    <t>jmoses@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +443,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00627A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -576,7 +809,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -584,6 +817,8 @@
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -906,17 +1141,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1022,185 +1257,411 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="8"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="3"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A57" s="3"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A59" s="3"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A61" s="3"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A62" s="3"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A63" s="3"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A64" s="3"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A65" s="3"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A66" s="3"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A67" s="3"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A69" s="3"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A71" s="3"/>
+      <c r="B92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1208,8 +1669,23 @@
     <hyperlink ref="A4" r:id="rId2"/>
     <hyperlink ref="A8" r:id="rId3" display="testmail1@test.com"/>
     <hyperlink ref="A9" r:id="rId4" display="testmail2@test.com"/>
+    <hyperlink ref="C92" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>